<commit_message>
Commit atualização imagens e posts
</commit_message>
<xml_diff>
--- a/insta_clip/data/posts.xlsx
+++ b/insta_clip/data/posts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srest\PycharmProjects\insta_clip\insta_clip\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A34436-38A5-45B8-9593-8C4A6F99B569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6B44CF-1BF6-45C8-8ACA-4ABF1CC1148A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="582">
   <si>
     <t>post_id</t>
   </si>
@@ -1868,6 +1868,94 @@
   </si>
   <si>
     <t>/static/images/jose_simoes_post_2.jpeg</t>
+  </si>
+  <si>
+    <t>ELEIÇÕES FILTO 2024: CHEGOU A HORA DE DECIDIR O FUTURO DA NOSSA REGIÃO. 🗳️
+Entre 03 e 07 de novembro, vocês vão às urnas para escolher quem vai liderar a FILTO nos próximos anos. E essa NÃO é uma eleição qualquer. É uma decisão sobre QUE CAMINHO queremos seguir.
+Há quem prefira recuar. Moderar o tom. Abandonar quem ainda luta pela LIBERDADE e pela PROSPERIDADE que nos foi negada por décadas.
+EU ESCOLHI OUTRO CAMINHO.
+Desde que assumi a presidência da FILTO, deixei claro: não haverá prosperidade econômica e social real na nossa região enquanto PERUÍBE não for LIVRE.
+E isso significa MANTER NOSSO COMPROMISSO com o MPL. Significa continuar financiando a luta pela independência até que ela se CONCRETIZE.
+Meu oponente, Tobias Inácio Neto, vem fazendo campanha com discurso "moderado". Bonito nas palavras, vazio nas ações. Ele diz que "pujança econômica não vem de ações armadas".
+EU DIGO O CONTRÁRIO:
+Pujança econômica não vem de submissão. Não vem de aceitar migalhas. Não vem de negociar nossa dignidade em mesas onde NUNCA fomos respeitados.
+A história mostra: povos que conquistaram sua autodeterminação LUTARAM por ela. E nós não seremos exceção.</t>
+  </si>
+  <si>
+    <t>rodrigo_abelardo</t>
+  </si>
+  <si>
+    <t>Rodrigo Velásquez Abelardo</t>
+  </si>
+  <si>
+    <t>Rodrigo Velásquez Abelardo
+Presidente da FILTO | Candidato à Reeleição
+Federação dos Interesses de TOPÁZIO
+Compromisso com PERUÍBE LIVRE
+Prosperidade vem da liberdade, não da submissão
+📍 Região de Peruíbe - TOPÁZIO</t>
+  </si>
+  <si>
+    <t>ELEIÇÕES FILTO 2024: É HORA DE ESCOLHER O FUTURO COM RESPONSABILIDADE. 🗳️
+Entre 03 e 07 de novembro, nossa região decide os rumos da FILTO. E essa decisão vai além de discursos inflamados ou promessas vazias. É sobre RESULTADOS REAIS para quem vive, trabalha e constrói aqui todos os dias.
+Meu adversário, Rodrigo Velásquez Abelardo, quer continuar comprometendo recursos da federação com financiamento indefinido ao MPL. Ele acredita que prosperidade vem de "ações armadas" e confronto permanente.
+EU ACREDITO EM OUTRO CAMINHO.
+Acredito que a PUJANÇA ECONÔMICA da nossa região não pode depender de conflitos que drenam nossos recursos, afastam investimentos e colocam vidas em risco.</t>
+  </si>
+  <si>
+    <t>Tobias Inácio Neto</t>
+  </si>
+  <si>
+    <t>tobias_inacio</t>
+  </si>
+  <si>
+    <t>Tobias Inácio Neto
+Candidato a Presidente da FILTO
+Federação dos Interesses de TOPÁZIO
+Desenvolvimento real, prosperidade com paz
+Mudança responsável para nossa região</t>
+  </si>
+  <si>
+    <t>/static/images/rodrigo_abelardo_post_1.png</t>
+  </si>
+  <si>
+    <t>/static/images/tobias_inacio_post_1.png</t>
+  </si>
+  <si>
+    <t>Lucas Santos
+2º Secretário Executivo | FILTO
+Controle Financeiro Interino
+Gestão transparente e responsável
+Alinhado com Tobias Inácio Neto
+Os números não mentem
+📊 Federação TOPÁZIO
+📍 Região de Peruíbe</t>
+  </si>
+  <si>
+    <t>lucas_santos</t>
+  </si>
+  <si>
+    <t>Lucas Santos</t>
+  </si>
+  <si>
+    <t>Como 2º Secretário Executivo, acabo de assumir INTERINAMENTE o controle financeiro da FILTO. E o que encontrei precisa ser dito com CLAREZA.
+Nos últimos anos, nossa federação comprometeu MILHÕES em financiamento ao MPL. Recursos que saem dos nossos associados, das nossas empresas, do suor de quem trabalha nesta região.
+E o retorno? Onde está a prosperidade prometida?
+VAMOS AOS NÚMEROS:
+Enquanto despejamos recursos em "ações estratégicas" e "apoio logístico ao movimento", temos:
+❌ Escolas sem reforma há anos
+❌ Estradas em condições precárias
+❌ Pequenos produtores sem crédito
+❌ Jovens sem perspectiva de emprego
+❌ Infraestrutura sucateada
+NÃO É SUSTENTÁVEL. NÃO É INTELIGENTE.
+Como gestor financeiro, minha responsabilidade é com os NÚMEROS, não com discursos. E os números mostram uma federação SANGRANDO recursos para um projeto sem fim definido.
+Entre 03 e 07 de novembro, vocês vão decidir: continuamos nessa espiral de dependência e desperdício, ou mudamos o rumo?
+MINHA POSIÇÃO É TÉCNICA, MAS TAMBÉM É POLÍTICA:
+Alinho-me com a candidatura de TOBIAS INÁCIO NETO porque acredito em gestão RESPONSÁVEL. Porque acredito que prosperidade se constrói com INVESTIMENTO PRODUTIVO, não com cheques em branco para conflitos sem horizonte.</t>
+  </si>
+  <si>
+    <t>/static/images/lucas_santos_post_1.png</t>
   </si>
 </sst>
 </file>
@@ -2376,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4474,15 +4562,15 @@
       </c>
       <c r="K31">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>38560</v>
+        <v>67480</v>
       </c>
       <c r="L31">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>14460</v>
+        <v>19280</v>
       </c>
       <c r="M31">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>14460</v>
+        <v>4820</v>
       </c>
       <c r="N31"/>
       <c r="O31"/>
@@ -4528,11 +4616,11 @@
       </c>
       <c r="K32">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>34580</v>
+        <v>27170</v>
       </c>
       <c r="L32">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>14820</v>
+        <v>9880</v>
       </c>
       <c r="M32">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -4586,7 +4674,7 @@
       </c>
       <c r="L33">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>6150</v>
+        <v>10250</v>
       </c>
       <c r="M33">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -4637,11 +4725,11 @@
       </c>
       <c r="L34">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>568</v>
+        <v>426</v>
       </c>
       <c r="M34">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>284</v>
+        <v>142</v>
       </c>
       <c r="N34"/>
       <c r="O34"/>
@@ -4684,15 +4772,15 @@
       </c>
       <c r="K35">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>923</v>
+        <v>994</v>
       </c>
       <c r="L35">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>497</v>
+      </c>
+      <c r="M35">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
         <v>213</v>
-      </c>
-      <c r="M35">
-        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>71</v>
       </c>
       <c r="N35"/>
       <c r="O35"/>
@@ -4738,15 +4826,15 @@
       </c>
       <c r="K36">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>15900</v>
+        <v>22260</v>
       </c>
       <c r="L36">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>6360</v>
+        <v>19080</v>
       </c>
       <c r="M36">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>15900</v>
+        <v>3180</v>
       </c>
       <c r="N36"/>
       <c r="O36"/>
@@ -4789,7 +4877,7 @@
       </c>
       <c r="K37">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>1204</v>
+        <v>774</v>
       </c>
       <c r="L37">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
@@ -4797,7 +4885,7 @@
       </c>
       <c r="M37">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>344</v>
+        <v>86</v>
       </c>
       <c r="N37"/>
       <c r="O37"/>
@@ -4840,15 +4928,15 @@
       </c>
       <c r="K38">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>32880</v>
+        <v>19180</v>
       </c>
       <c r="L38">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>13700</v>
+        <v>5480</v>
       </c>
       <c r="M38">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>13700</v>
+        <v>2740</v>
       </c>
       <c r="N38"/>
       <c r="O38"/>
@@ -4891,15 +4979,15 @@
       </c>
       <c r="K39">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>30140</v>
+        <v>24660</v>
       </c>
       <c r="L39">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>21920</v>
+        <v>5480</v>
       </c>
       <c r="M39">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>2740</v>
+        <v>13700</v>
       </c>
       <c r="N39"/>
       <c r="O39"/>
@@ -4942,15 +5030,15 @@
       </c>
       <c r="K40">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>384</v>
+        <v>576</v>
       </c>
       <c r="L40">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>384</v>
+        <v>448</v>
       </c>
       <c r="M40">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="N40"/>
       <c r="O40"/>
@@ -4996,15 +5084,15 @@
       </c>
       <c r="K41">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>10990</v>
+        <v>11775</v>
       </c>
       <c r="L41">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>6280</v>
+        <v>1570</v>
       </c>
       <c r="M41">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>1570</v>
+        <v>2355</v>
       </c>
       <c r="N41"/>
       <c r="O41"/>
@@ -5047,7 +5135,7 @@
       </c>
       <c r="K42">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>920</v>
+        <v>1104</v>
       </c>
       <c r="L42">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
@@ -5055,7 +5143,7 @@
       </c>
       <c r="M42">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>368</v>
+        <v>184</v>
       </c>
       <c r="N42"/>
       <c r="O42"/>
@@ -5101,11 +5189,11 @@
       </c>
       <c r="K43">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>2431</v>
+        <v>2618</v>
       </c>
       <c r="L43">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>374</v>
+        <v>561</v>
       </c>
       <c r="M43">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -5152,7 +5240,7 @@
       </c>
       <c r="K44">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>1419</v>
+        <v>903</v>
       </c>
       <c r="L44">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
@@ -5160,7 +5248,7 @@
       </c>
       <c r="M44">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>645</v>
+        <v>516</v>
       </c>
       <c r="N44"/>
       <c r="O44"/>
@@ -5203,15 +5291,15 @@
       </c>
       <c r="K45">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>168000</v>
+        <v>108000</v>
       </c>
       <c r="L45">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>36000</v>
+        <v>48000</v>
       </c>
       <c r="M45">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>60000</v>
+        <v>12000</v>
       </c>
       <c r="N45"/>
       <c r="O45"/>
@@ -5251,15 +5339,15 @@
       </c>
       <c r="K46">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>372000</v>
+        <v>248000</v>
       </c>
       <c r="L46">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>217000</v>
+        <v>248000</v>
       </c>
       <c r="M46">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>93000</v>
+        <v>31000</v>
       </c>
       <c r="N46"/>
       <c r="O46"/>
@@ -5302,15 +5390,15 @@
       </c>
       <c r="K47">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>102000</v>
+        <v>42500</v>
       </c>
       <c r="L47">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>68000</v>
+        <v>34000</v>
       </c>
       <c r="M47">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>42500</v>
+        <v>17000</v>
       </c>
       <c r="N47"/>
       <c r="O47"/>
@@ -5353,15 +5441,15 @@
       </c>
       <c r="K48">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>60000</v>
+        <v>54000</v>
       </c>
       <c r="L48">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>36000</v>
+        <v>30000</v>
       </c>
       <c r="M48">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>30000</v>
+        <v>12000</v>
       </c>
       <c r="N48"/>
       <c r="O48"/>
@@ -5404,15 +5492,15 @@
       </c>
       <c r="K49">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>72000</v>
+        <v>66000</v>
       </c>
       <c r="L49">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>24000</v>
+        <v>12000</v>
       </c>
       <c r="M49">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>24000</v>
+        <v>18000</v>
       </c>
       <c r="N49"/>
       <c r="O49"/>
@@ -5462,11 +5550,11 @@
       </c>
       <c r="L50">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>4600</v>
+        <v>6900</v>
       </c>
       <c r="M50">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>4600</v>
+        <v>2300</v>
       </c>
       <c r="N50"/>
       <c r="O50"/>
@@ -5512,15 +5600,15 @@
       </c>
       <c r="K51">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>29900</v>
+        <v>16100</v>
       </c>
       <c r="L51">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>11500</v>
+        <v>18400</v>
       </c>
       <c r="M51">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>11500</v>
+        <v>6900</v>
       </c>
       <c r="N51"/>
       <c r="O51"/>
@@ -5566,11 +5654,11 @@
       </c>
       <c r="K52">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>16116</v>
+        <v>34533</v>
       </c>
       <c r="L52">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>13813</v>
+        <v>6907</v>
       </c>
       <c r="M52">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -5621,7 +5709,7 @@
       </c>
       <c r="L53">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>248000</v>
+        <v>93000</v>
       </c>
       <c r="M53">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -5668,15 +5756,15 @@
       </c>
       <c r="K54">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>156000</v>
+        <v>132000</v>
       </c>
       <c r="L54">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>48000</v>
+        <v>24000</v>
       </c>
       <c r="M54">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>12000</v>
+        <v>24000</v>
       </c>
       <c r="N54"/>
       <c r="O54"/>
@@ -5719,11 +5807,11 @@
       </c>
       <c r="K55">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>57840</v>
+        <v>48200</v>
       </c>
       <c r="L55">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>9640</v>
+        <v>24100</v>
       </c>
       <c r="M55">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -5770,15 +5858,15 @@
       </c>
       <c r="K56">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>935</v>
+        <v>2057</v>
       </c>
       <c r="L56">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>748</v>
+        <v>374</v>
       </c>
       <c r="M56">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>935</v>
+        <v>561</v>
       </c>
       <c r="N56"/>
       <c r="O56"/>
@@ -5818,15 +5906,15 @@
       </c>
       <c r="K57">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>645</v>
+      </c>
+      <c r="L57">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
         <v>1032</v>
       </c>
-      <c r="L57">
-        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>258</v>
-      </c>
       <c r="M57">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>387</v>
+        <v>516</v>
       </c>
       <c r="N57"/>
       <c r="O57"/>
@@ -5869,15 +5957,15 @@
       </c>
       <c r="K58">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>34580</v>
+        <v>27170</v>
       </c>
       <c r="L58">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>19760</v>
+      </c>
+      <c r="M58">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
         <v>7410</v>
-      </c>
-      <c r="M58">
-        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>12350</v>
       </c>
       <c r="N58"/>
       <c r="O58"/>
@@ -5920,15 +6008,15 @@
       </c>
       <c r="K59">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>18450</v>
+        <v>14350</v>
       </c>
       <c r="L59">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>14350</v>
+        <v>4100</v>
       </c>
       <c r="M59">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>6150</v>
+        <v>4100</v>
       </c>
       <c r="N59"/>
       <c r="O59"/>
@@ -5968,7 +6056,7 @@
       </c>
       <c r="K60">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>781</v>
+        <v>355</v>
       </c>
       <c r="L60">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
@@ -5976,7 +6064,7 @@
       </c>
       <c r="M60">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>284</v>
+        <v>71</v>
       </c>
       <c r="N60"/>
       <c r="O60"/>
@@ -6019,15 +6107,15 @@
       </c>
       <c r="K61">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>34980</v>
+        <v>22260</v>
       </c>
       <c r="L61">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>9540</v>
+        <v>25440</v>
       </c>
       <c r="M61">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>6360</v>
+        <v>12720</v>
       </c>
       <c r="N61"/>
       <c r="O61"/>
@@ -6067,7 +6155,7 @@
       </c>
       <c r="K62">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>1118</v>
+        <v>1204</v>
       </c>
       <c r="L62">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
@@ -6075,7 +6163,7 @@
       </c>
       <c r="M62">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>430</v>
+        <v>172</v>
       </c>
       <c r="N62"/>
       <c r="O62"/>
@@ -6115,15 +6203,15 @@
       </c>
       <c r="K63">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>19180</v>
+      </c>
+      <c r="L63">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
         <v>13700</v>
       </c>
-      <c r="L63">
-        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>13700</v>
-      </c>
       <c r="M63">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>5480</v>
+        <v>2740</v>
       </c>
       <c r="N63"/>
       <c r="O63"/>
@@ -6171,7 +6259,7 @@
       </c>
       <c r="M64">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="N64"/>
       <c r="O64"/>
@@ -6214,15 +6302,15 @@
       </c>
       <c r="K65">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>8635</v>
+        <v>10205</v>
       </c>
       <c r="L65">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>6280</v>
+        <v>3140</v>
       </c>
       <c r="M65">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>3925</v>
+        <v>1570</v>
       </c>
       <c r="N65"/>
       <c r="O65"/>
@@ -6262,15 +6350,15 @@
       </c>
       <c r="K66">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>828</v>
+        <v>460</v>
       </c>
       <c r="L66">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>644</v>
+        <v>460</v>
       </c>
       <c r="M66">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>460</v>
+        <v>92</v>
       </c>
       <c r="N66"/>
       <c r="O66"/>
@@ -6313,11 +6401,11 @@
       </c>
       <c r="K67">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>156000</v>
+        <v>108000</v>
       </c>
       <c r="L67">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>84000</v>
+        <v>48000</v>
       </c>
       <c r="M67">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
@@ -6361,15 +6449,15 @@
       </c>
       <c r="K68">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>341000</v>
+        <v>403000</v>
       </c>
       <c r="L68">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>93000</v>
+        <v>248000</v>
       </c>
       <c r="M68">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>155000</v>
+        <v>31000</v>
       </c>
       <c r="N68"/>
       <c r="O68"/>
@@ -6412,15 +6500,15 @@
       </c>
       <c r="K69">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>102000</v>
+        <v>59500</v>
       </c>
       <c r="L69">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>68000</v>
+        <v>51000</v>
       </c>
       <c r="M69">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>42500</v>
+        <v>25500</v>
       </c>
       <c r="N69"/>
       <c r="O69"/>
@@ -6463,15 +6551,15 @@
       </c>
       <c r="K70">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>18400</v>
+        <v>13800</v>
       </c>
       <c r="L70">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>13800</v>
+        <v>4600</v>
       </c>
       <c r="M70">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>4600</v>
+        <v>9200</v>
       </c>
       <c r="N70"/>
       <c r="O70"/>
@@ -6517,15 +6605,15 @@
       </c>
       <c r="K71">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
-        <v>403000</v>
+        <v>310000</v>
       </c>
       <c r="L71">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>186000</v>
+        <v>93000</v>
       </c>
       <c r="M71">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>155000</v>
+        <v>31000</v>
       </c>
       <c r="N71"/>
       <c r="O71"/>
@@ -6575,11 +6663,11 @@
       </c>
       <c r="L72">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>60000</v>
+      </c>
+      <c r="M72">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
         <v>48000</v>
-      </c>
-      <c r="M72">
-        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>24000</v>
       </c>
       <c r="N72"/>
       <c r="O72"/>
@@ -6626,11 +6714,11 @@
       </c>
       <c r="L73">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="M73">
         <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:23" ht="409.6" x14ac:dyDescent="0.3">
@@ -6662,40 +6750,139 @@
         <v>45958.666666666664</v>
       </c>
       <c r="K74">
-        <v>78</v>
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>65</v>
       </c>
       <c r="L74">
-        <v>20</v>
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>91</v>
       </c>
       <c r="M74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>126</v>
       </c>
-      <c r="E75" s="1"/>
+      <c r="B75" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="F75">
+        <v>1300</v>
+      </c>
+      <c r="G75">
+        <v>110</v>
+      </c>
+      <c r="H75" t="s">
+        <v>575</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>567</v>
+      </c>
       <c r="J75" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>195</v>
+      </c>
+      <c r="L75">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>52</v>
+      </c>
+      <c r="M75">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" ht="255.75" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>127</v>
       </c>
-      <c r="E76" s="1"/>
+      <c r="B76" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F76">
+        <v>1300</v>
+      </c>
+      <c r="G76">
+        <v>110</v>
+      </c>
+      <c r="H76" t="s">
+        <v>576</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>571</v>
+      </c>
       <c r="J76" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>156</v>
+      </c>
+      <c r="L76">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>52</v>
+      </c>
+      <c r="M76">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>128</v>
       </c>
-      <c r="E77" s="1"/>
+      <c r="B77" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F77">
+        <v>362</v>
+      </c>
+      <c r="G77">
+        <v>112</v>
+      </c>
+      <c r="H77" t="s">
+        <v>581</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>580</v>
+      </c>
       <c r="J77" s="4">
         <v>45958.666666666664</v>
+      </c>
+      <c r="K77">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>36</v>
+      </c>
+      <c r="L77">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>7</v>
+      </c>
+      <c r="M77">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -6706,6 +6893,18 @@
       <c r="J78" s="4">
         <v>45958.666666666664</v>
       </c>
+      <c r="K78">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -6715,6 +6914,18 @@
       <c r="J79" s="4">
         <v>45958.666666666664</v>
       </c>
+      <c r="K79">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -6724,8 +6935,20 @@
       <c r="J80" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>132</v>
       </c>
@@ -6733,8 +6956,20 @@
       <c r="J81" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>133</v>
       </c>
@@ -6742,8 +6977,20 @@
       <c r="J82" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>134</v>
       </c>
@@ -6751,8 +6998,20 @@
       <c r="J83" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>135</v>
       </c>
@@ -6760,8 +7019,20 @@
       <c r="J84" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>136</v>
       </c>
@@ -6769,8 +7040,20 @@
       <c r="J85" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>137</v>
       </c>
@@ -6778,8 +7061,20 @@
       <c r="J86" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>138</v>
       </c>
@@ -6787,8 +7082,20 @@
       <c r="J87" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>139</v>
       </c>
@@ -6796,8 +7103,20 @@
       <c r="J88" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>140</v>
       </c>
@@ -6805,8 +7124,20 @@
       <c r="J89" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -6814,8 +7145,20 @@
       <c r="J90" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>142</v>
       </c>
@@ -6823,8 +7166,20 @@
       <c r="J91" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -6832,8 +7187,20 @@
       <c r="J92" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>144</v>
       </c>
@@ -6841,8 +7208,20 @@
       <c r="J93" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>145</v>
       </c>
@@ -6850,8 +7229,20 @@
       <c r="J94" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>146</v>
       </c>
@@ -6859,8 +7250,20 @@
       <c r="J95" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>147</v>
       </c>
@@ -6868,8 +7271,20 @@
       <c r="J96" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>148</v>
       </c>
@@ -6877,8 +7292,20 @@
       <c r="J97" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>149</v>
       </c>
@@ -6886,8 +7313,20 @@
       <c r="J98" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>150</v>
       </c>
@@ -6895,8 +7334,20 @@
       <c r="J99" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>151</v>
       </c>
@@ -6904,8 +7355,20 @@
       <c r="J100" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K100">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>152</v>
       </c>
@@ -6913,8 +7376,20 @@
       <c r="J101" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>153</v>
       </c>
@@ -6922,8 +7397,20 @@
       <c r="J102" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K102">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -6931,8 +7418,20 @@
       <c r="J103" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>155</v>
       </c>
@@ -6940,8 +7439,20 @@
       <c r="J104" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K104">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>156</v>
       </c>
@@ -6949,8 +7460,20 @@
       <c r="J105" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K105">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>157</v>
       </c>
@@ -6958,8 +7481,20 @@
       <c r="J106" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K106">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>158</v>
       </c>
@@ -6967,8 +7502,20 @@
       <c r="J107" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K107">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>159</v>
       </c>
@@ -6976,8 +7523,20 @@
       <c r="J108" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>160</v>
       </c>
@@ -6985,8 +7544,20 @@
       <c r="J109" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K109">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M109">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>161</v>
       </c>
@@ -6994,8 +7565,20 @@
       <c r="J110" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K110">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>162</v>
       </c>
@@ -7003,8 +7586,20 @@
       <c r="J111" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K111">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>163</v>
       </c>
@@ -7012,8 +7607,20 @@
       <c r="J112" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K112">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>164</v>
       </c>
@@ -7021,8 +7628,20 @@
       <c r="J113" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>165</v>
       </c>
@@ -7030,8 +7649,20 @@
       <c r="J114" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K114">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>166</v>
       </c>
@@ -7039,8 +7670,20 @@
       <c r="J115" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K115">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>167</v>
       </c>
@@ -7048,8 +7691,20 @@
       <c r="J116" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K116">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M116">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>168</v>
       </c>
@@ -7057,8 +7712,20 @@
       <c r="J117" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M117">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>169</v>
       </c>
@@ -7066,8 +7733,20 @@
       <c r="J118" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K118">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>170</v>
       </c>
@@ -7075,8 +7754,20 @@
       <c r="J119" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K119">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>171</v>
       </c>
@@ -7084,8 +7775,20 @@
       <c r="J120" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K120">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>172</v>
       </c>
@@ -7093,8 +7796,20 @@
       <c r="J121" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K121">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>173</v>
       </c>
@@ -7102,8 +7817,20 @@
       <c r="J122" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K122">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>174</v>
       </c>
@@ -7111,8 +7838,20 @@
       <c r="J123" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>175</v>
       </c>
@@ -7120,8 +7859,20 @@
       <c r="J124" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>176</v>
       </c>
@@ -7129,8 +7880,20 @@
       <c r="J125" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K125">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>177</v>
       </c>
@@ -7138,8 +7901,20 @@
       <c r="J126" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K126">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>178</v>
       </c>
@@ -7147,14 +7922,38 @@
       <c r="J127" s="4">
         <v>45958.666666666664</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>179</v>
       </c>
       <c r="E128" s="1"/>
       <c r="J128" s="4">
         <v>45958.666666666664</v>
+      </c>
+      <c r="K128">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(5,15) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(2,8) / 100), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <f ca="1">ROUND(Tabela1[[#This Row],[actor_followers]] * (RANDBETWEEN(1,5) / 100), 0)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>